<commit_message>
Updated model, more configurations and environments
</commit_message>
<xml_diff>
--- a/Configuration/Environment database.xlsx
+++ b/Configuration/Environment database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\python\Covid-Building-Infections\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46742852-11F5-4DDA-B4D0-7477D010712B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EC386C-6F26-4297-9FF1-E904D272D2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25515" yWindow="840" windowWidth="23670" windowHeight="14220" xr2:uid="{E0B6F48B-B433-4215-88BE-0678B68CE95E}"/>
+    <workbookView xWindow="-25740" yWindow="1200" windowWidth="23670" windowHeight="14220" xr2:uid="{E0B6F48B-B433-4215-88BE-0678B68CE95E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>volume</t>
   </si>
@@ -138,13 +138,60 @@
   </si>
   <si>
     <t>Bank-mechanical-Lockdown</t>
+  </si>
+  <si>
+    <t>Lounge-Two People-Winter-15 Mins</t>
+  </si>
+  <si>
+    <t>Lounge-Two People-Winter-30 Mins</t>
+  </si>
+  <si>
+    <t>Lounge-Two People-Winter-1 hour</t>
+  </si>
+  <si>
+    <t>Lounge-Two People-Summer-15 Mins</t>
+  </si>
+  <si>
+    <t>Lounge-Two People-Summer-30 Mins</t>
+  </si>
+  <si>
+    <t>Lounge-Two People-Summer-1 hour</t>
+  </si>
+  <si>
+    <t>Lounge-Four People-Winter-15 Mins</t>
+  </si>
+  <si>
+    <t>Lounge-Four People-Winter-30 Mins</t>
+  </si>
+  <si>
+    <t>Lounge-Four People-Winter-1 hour</t>
+  </si>
+  <si>
+    <t>Lounge-Four People-Summer-15 Mins</t>
+  </si>
+  <si>
+    <t>Lounge-Four People-Summer-30 Mins</t>
+  </si>
+  <si>
+    <t>Lounge-Four People-Summer-1 hour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,16 +217,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -492,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A2E0E55-67AE-4901-9E6A-ACA877836B25}">
-  <dimension ref="A2:J23"/>
+  <dimension ref="A2:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27:J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +642,7 @@
       <c r="I6" s="1">
         <v>5</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="2">
         <v>0.2</v>
       </c>
     </row>
@@ -623,7 +675,7 @@
       <c r="I7" s="1">
         <v>5</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="2">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -656,7 +708,7 @@
       <c r="I8" s="1">
         <v>5</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="2">
         <v>0.2</v>
       </c>
     </row>
@@ -689,7 +741,7 @@
       <c r="I9" s="1">
         <v>5</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="2">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -701,7 +753,7 @@
         <v>1800</v>
       </c>
       <c r="C10" s="1">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -710,19 +762,18 @@
         <v>0</v>
       </c>
       <c r="F10" s="1">
-        <f>1/120</f>
-        <v>8.3333333333333332E-3</v>
+        <v>0.5</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <v>60</v>
+        <v>100000</v>
       </c>
       <c r="I10" s="1">
         <v>10</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="2">
         <v>0.2</v>
       </c>
     </row>
@@ -734,7 +785,7 @@
         <v>1800</v>
       </c>
       <c r="C11" s="1">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -743,19 +794,18 @@
         <v>0</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" ref="F11:F13" si="0">1/120</f>
-        <v>8.3333333333333332E-3</v>
+        <v>0.5</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <v>60</v>
+        <v>100000</v>
       </c>
       <c r="I11" s="1">
         <v>10</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="2">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -767,7 +817,7 @@
         <v>1800</v>
       </c>
       <c r="C12" s="1">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -776,8 +826,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333332E-3</v>
+        <v>0.5</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
@@ -788,7 +837,7 @@
       <c r="I12" s="1">
         <v>10</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="2">
         <v>0.2</v>
       </c>
     </row>
@@ -800,7 +849,7 @@
         <v>1800</v>
       </c>
       <c r="C13" s="1">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -809,8 +858,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333332E-3</v>
+        <v>0.5</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
@@ -821,7 +869,7 @@
       <c r="I13" s="1">
         <v>10</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="2">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -853,7 +901,7 @@
       <c r="I14" s="1">
         <v>4</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="2">
         <v>0.2</v>
       </c>
     </row>
@@ -885,7 +933,7 @@
       <c r="I15" s="1">
         <v>4</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="2">
         <v>9.6</v>
       </c>
     </row>
@@ -917,7 +965,7 @@
       <c r="I16" s="1">
         <v>8</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="2">
         <v>0.2</v>
       </c>
     </row>
@@ -949,7 +997,7 @@
       <c r="I17" s="1">
         <v>8</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="2">
         <v>2.4</v>
       </c>
     </row>
@@ -961,7 +1009,7 @@
         <v>300</v>
       </c>
       <c r="C18" s="1">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -982,7 +1030,7 @@
       <c r="I18" s="1">
         <v>8</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="2">
         <v>0.5</v>
       </c>
     </row>
@@ -994,7 +1042,7 @@
         <v>300</v>
       </c>
       <c r="C19" s="1">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -1015,7 +1063,7 @@
       <c r="I19" s="1">
         <v>8</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="2">
         <v>2.4</v>
       </c>
     </row>
@@ -1047,7 +1095,7 @@
       <c r="I20" s="1">
         <v>4</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="2">
         <v>0.2</v>
       </c>
     </row>
@@ -1079,7 +1127,7 @@
       <c r="I21" s="1">
         <v>4</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21" s="2">
         <v>2.4</v>
       </c>
     </row>
@@ -1091,7 +1139,7 @@
         <v>100</v>
       </c>
       <c r="C22" s="1">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -1112,7 +1160,7 @@
       <c r="I22" s="1">
         <v>4</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22" s="2">
         <v>0.5</v>
       </c>
     </row>
@@ -1124,7 +1172,7 @@
         <v>100</v>
       </c>
       <c r="C23" s="1">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -1145,8 +1193,404 @@
       <c r="I23" s="1">
         <v>4</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="2">
         <v>2.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" ref="B24:B35" si="0">4*3*2.7</f>
+        <v>32.400000000000006</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>2</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="0"/>
+        <v>32.400000000000006</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>2</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="1">
+        <f t="shared" si="0"/>
+        <v>32.400000000000006</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>2</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>2</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" si="0"/>
+        <v>32.400000000000006</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>2</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>2</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" si="0"/>
+        <v>32.400000000000006</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>2</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>2</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="0"/>
+        <v>32.400000000000006</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>2</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" si="0"/>
+        <v>32.400000000000006</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>4</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>4</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="0"/>
+        <v>32.400000000000006</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>4</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>4</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="0"/>
+        <v>32.400000000000006</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>4</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>4</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="0"/>
+        <v>32.400000000000006</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>4</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
+        <v>4</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="0"/>
+        <v>32.400000000000006</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>4</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>4</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+      <c r="J34" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="0"/>
+        <v>32.400000000000006</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>4</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>4</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>